<commit_message>
Create graphs for Claudia
</commit_message>
<xml_diff>
--- a/Rodent Traps/RodentTrap_MasterRecords.xlsx
+++ b/Rodent Traps/RodentTrap_MasterRecords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nolagov-my.sharepoint.com/personal/mark_myer_nola_gov/Documents/Rodent Surveillance/Rodent Traps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{88C5B815-2601-124E-A614-11FDF9BECCF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A22B62FF-4491-419A-A9FC-914C08B5E66B}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{88C5B815-2601-124E-A614-11FDF9BECCF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ECABDD5C-2ABA-4992-B08F-8A3090078E4A}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="15660" windowHeight="17440" xr2:uid="{D1D549A4-2765-1F41-8DEB-9ED227E36AD3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="28">
   <si>
     <t>Location</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>F?</t>
   </si>
   <si>
     <t>FM</t>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D859642C-4E80-9743-B87C-25FADBC42825}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -920,6 +926,184 @@
       </c>
       <c r="E25">
         <v>3095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1">
+        <v>43966</v>
+      </c>
+      <c r="D26">
+        <v>3091</v>
+      </c>
+      <c r="E26">
+        <v>3042</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="1">
+        <v>43966</v>
+      </c>
+      <c r="D27">
+        <v>3054</v>
+      </c>
+      <c r="E27">
+        <v>3018</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="1">
+        <v>43966</v>
+      </c>
+      <c r="D28">
+        <v>3046</v>
+      </c>
+      <c r="E28">
+        <v>3041</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="1">
+        <v>43966</v>
+      </c>
+      <c r="D29">
+        <v>3085</v>
+      </c>
+      <c r="E29">
+        <v>3084</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="1">
+        <v>43966</v>
+      </c>
+      <c r="D30">
+        <v>3078</v>
+      </c>
+      <c r="E30">
+        <v>3087</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1">
+        <v>43966</v>
+      </c>
+      <c r="D31">
+        <v>3012</v>
+      </c>
+      <c r="E31">
+        <v>3039</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1">
+        <v>43966</v>
+      </c>
+      <c r="D32">
+        <v>3098</v>
+      </c>
+      <c r="E32">
+        <v>3044</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1">
+        <v>43967</v>
+      </c>
+      <c r="D33">
+        <v>3087</v>
+      </c>
+      <c r="E33">
+        <v>3003</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1">
+        <v>43967</v>
+      </c>
+      <c r="D34">
+        <v>3084</v>
+      </c>
+      <c r="E34">
+        <v>3038</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="1">
+        <v>43967</v>
+      </c>
+      <c r="D35">
+        <v>3041</v>
+      </c>
+      <c r="E35">
+        <v>3026</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="D36">
+        <v>3052</v>
+      </c>
+      <c r="E36">
+        <v>3037</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -939,18 +1123,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -958,23 +1142,23 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -982,7 +1166,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>